<commit_message>
Collelongo e test prime funzioni
</commit_message>
<xml_diff>
--- a/data-raw/sites_list.xlsx
+++ b/data-raw/sites_list.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ITINERIS-EVsVRE\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ITINERIS\Server\ITINERIS-EVsVRE\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D85DABC-E809-4310-9F36-D0F5FC34C9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94FD7C6-090D-4EDE-86BE-F864004CEDA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="15540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LTER_sites" sheetId="1" r:id="rId1"/>
     <sheet name="EV" sheetId="2" r:id="rId2"/>
     <sheet name="datasets" sheetId="3" r:id="rId3"/>
+    <sheet name="Sites_EBVDataPortal" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="165">
   <si>
     <t>https://deims.org/f30007c4-8a6e-4f11-ab87-569db54638fe</t>
   </si>
@@ -517,12 +518,165 @@
   <si>
     <t>collelongo</t>
   </si>
+  <si>
+    <t>id_ev</t>
+  </si>
+  <si>
+    <t>name_dp</t>
+  </si>
+  <si>
+    <t>id_dp</t>
+  </si>
+  <si>
+    <t>name_ev</t>
+  </si>
+  <si>
+    <t>Local bird diversity (cSAR/BES-SIM)</t>
+  </si>
+  <si>
+    <t>Forest loss from 2000 to 2020</t>
+  </si>
+  <si>
+    <t>Predicted suitability for EUNIS habitat types</t>
+  </si>
+  <si>
+    <t>Relative Magnitude of Fragmentation (RMF)</t>
+  </si>
+  <si>
+    <t>Global habitat availability for mammals from 2015-2055</t>
+  </si>
+  <si>
+    <t>Local terrestrial diversity (PREDICTS)</t>
+  </si>
+  <si>
+    <t>Habitat availability for African great apes</t>
+  </si>
+  <si>
+    <t>Global forest cover 2000</t>
+  </si>
+  <si>
+    <t>Vegetation Phenology in Finland</t>
+  </si>
+  <si>
+    <t>Canopy Chlorophyll Content for the Netherlands</t>
+  </si>
+  <si>
+    <t>Predicted suitability for EUNIS habitat types (100m resolution) for EU27 countries</t>
+  </si>
+  <si>
+    <t>Forest cover loss for Finland (e-shape, 0.00075 degrees)</t>
+  </si>
+  <si>
+    <t>Forest cover loss for Finland (e-shape, 0.0025 degrees)</t>
+  </si>
+  <si>
+    <t>Forest cover loss for Finland (e-shape, 0.0075 degrees)</t>
+  </si>
+  <si>
+    <t>Forest cover loss for Finland (e-shape, 0.025 degrees)</t>
+  </si>
+  <si>
+    <t>Forest cover loss for Finland (e-shape, 0.00025 degrees)</t>
+  </si>
+  <si>
+    <t>Global trends in biodiversity (BES-SIM GLOBIO)</t>
+  </si>
+  <si>
+    <t>Global trends in biodiversity (BES-SIM PREDICTS)</t>
+  </si>
+  <si>
+    <t>Global trends in biodiversity (BES-SIM cSAR-IIASA)</t>
+  </si>
+  <si>
+    <t>Global trends in biodiversity (BES-SIM cSAR-iDiv)</t>
+  </si>
+  <si>
+    <t>Global trends in biodiversity (BES-SIM AIM)</t>
+  </si>
+  <si>
+    <t>Tropical Andes macrogroup ecosystem extent</t>
+  </si>
+  <si>
+    <t>Tropical Andes formation ecosystem extent</t>
+  </si>
+  <si>
+    <t>Nocturnal bird migration across western Europe</t>
+  </si>
+  <si>
+    <t>Canopy Chlorophyll Content for the Bavarian Forest National Park</t>
+  </si>
+  <si>
+    <t>Historical local species richness (PREDICTS)</t>
+  </si>
+  <si>
+    <t>Net Primary Productivity for Bavarian Forest National Park</t>
+  </si>
+  <si>
+    <t>Net Primary Productivity in Europe 2015</t>
+  </si>
+  <si>
+    <t>Global trends in ecosystem services (BES-SIM LPJ-GUESS)</t>
+  </si>
+  <si>
+    <t>Global trends in ecosystem services (BES-SIM LPJ)</t>
+  </si>
+  <si>
+    <t>Global trends in ecosystem services (BES-SIM CABLE POP)</t>
+  </si>
+  <si>
+    <t>Global trends in ecosystem services (BES-SIM InVEST)</t>
+  </si>
+  <si>
+    <t>Global trends in ecosystem services (BES-SIM GLOBIO-ES)</t>
+  </si>
+  <si>
+    <t>Net Primary Productivity in Europe 2015 (monthly)</t>
+  </si>
+  <si>
+    <t>Tropical Andes species richness by macrogroup</t>
+  </si>
+  <si>
+    <t>Global trends in biodiversity (BES-SIM INSIGHTS) </t>
+  </si>
+  <si>
+    <t>Pasture production model</t>
+  </si>
+  <si>
+    <t>Post-fire legacies management and snow cover</t>
+  </si>
+  <si>
+    <t>Crop production for the Sierra Nevada National Park</t>
+  </si>
+  <si>
+    <t>Americas species richness by macrogroup </t>
+  </si>
+  <si>
+    <t>Distribution of European habitat types of the Habitats Directive (2018)</t>
+  </si>
+  <si>
+    <t>Distribution of European species of the Habitats Directive (2018)</t>
+  </si>
+  <si>
+    <t>Distribution of European bird species of the Birds Directive (2018)</t>
+  </si>
+  <si>
+    <t>Opportunity cost estimates for spatial conservation prioritisation across Europe</t>
+  </si>
+  <si>
+    <t>Breeding distribution of farmland birds (EBBA LIVE)</t>
+  </si>
+  <si>
+    <t>Occurrence Metrics for the Birds Directive Annex I Species in EU27: A 10 km prototype using GBIF occurrence cubes</t>
+  </si>
+  <si>
+    <t>Occurrence Metrics for Invasive Alien Species of Union Concern in EU27: A 10 km prototype using GBIF occurrence cubes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,6 +727,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -604,7 +764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -624,6 +784,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -931,7 +1092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1545,4 +1706,665 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D461525-DA5A-4C1D-AA1E-82B3B07C304E}">
+  <dimension ref="A1:D48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="108.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="str">
+        <f>+VLOOKUP(C2,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="9" t="str">
+        <f>+VLOOKUP(C3,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="9" t="e">
+        <f>+VLOOKUP(C4,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="9" t="e">
+        <f>+VLOOKUP(C5,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="9" t="e">
+        <f>+VLOOKUP(C6,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="9" t="str">
+        <f>+VLOOKUP(C7,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="9" t="str">
+        <f>+VLOOKUP(C8,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="9" t="str">
+        <f>+VLOOKUP(C9,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>10</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="9" t="str">
+        <f>+VLOOKUP(C10,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Terrestrial ecosystem phenology</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>13</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="9" t="e">
+        <f>+VLOOKUP(C11,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>15</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="9" t="e">
+        <f>+VLOOKUP(C12,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>22</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="9" t="str">
+        <f>+VLOOKUP(C13,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>23</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="9" t="str">
+        <f>+VLOOKUP(C14,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>24</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="9" t="str">
+        <f>+VLOOKUP(C15,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>25</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="9" t="str">
+        <f>+VLOOKUP(C16,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>26</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="9" t="str">
+        <f>+VLOOKUP(C17,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>27</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="9" t="e">
+        <f>+VLOOKUP(C18,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>28</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" s="9" t="e">
+        <f>+VLOOKUP(C19,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>29</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="9" t="e">
+        <f>+VLOOKUP(C20,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>30</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="9" t="e">
+        <f>+VLOOKUP(C21,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>31</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D22" s="9" t="e">
+        <f>+VLOOKUP(C22,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>34</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="9" t="str">
+        <f>+VLOOKUP(C23,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>38</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="9" t="str">
+        <f>+VLOOKUP(C24,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>42</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="9" t="str">
+        <f>+VLOOKUP(C25,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>53</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D26" s="9" t="e">
+        <f>+VLOOKUP(C26,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>55</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D27" s="9" t="e">
+        <f>+VLOOKUP(C27,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>58</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="9" t="str">
+        <f>+VLOOKUP(C28,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Terrestrial ecosystem productivity</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>59</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" s="9" t="e">
+        <f>+VLOOKUP(C29,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>60</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D30" s="9" t="e">
+        <f>+VLOOKUP(C30,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>61</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31" s="9" t="e">
+        <f>+VLOOKUP(C31,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>62</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D32" s="9" t="e">
+        <f>+VLOOKUP(C32,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>63</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="9" t="e">
+        <f>+VLOOKUP(C33,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>64</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34" s="9" t="e">
+        <f>+VLOOKUP(C34,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>66</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D35" s="9" t="e">
+        <f>+VLOOKUP(C35,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
+        <v>67</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="9" t="str">
+        <f>+VLOOKUP(C36,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>68</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D37" s="9" t="e">
+        <f>+VLOOKUP(C37,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>69</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" s="9" t="str">
+        <f>+VLOOKUP(C38,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Terrestrial ecosystem productivity</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>70</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D39" s="9" t="e">
+        <f>+VLOOKUP(C39,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>72</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="9" t="str">
+        <f>+VLOOKUP(C40,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Terrestrial ecosystem productivity</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>73</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D41" s="9" t="e">
+        <f>+VLOOKUP(C41,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>75</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D42" s="9" t="e">
+        <f>+VLOOKUP(C42,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>76</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D43" s="9" t="e">
+        <f>+VLOOKUP(C43,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
+        <v>77</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="9" t="str">
+        <f>+VLOOKUP(C44,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="9">
+        <v>78</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D45" s="9" t="e">
+        <f>+VLOOKUP(C45,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
+        <v>79</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="9" t="str">
+        <f>+VLOOKUP(C46,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="9">
+        <v>82</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C47" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="9" t="str">
+        <f>+VLOOKUP(C47,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>Species distributions of selected terrestrial plants</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="9">
+        <v>83</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D48" s="9" t="e">
+        <f>+VLOOKUP(C48,EV!$A$1:$B$14,2,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Prepare data presentation and storage
</commit_message>
<xml_diff>
--- a/data-raw/sites_list.xlsx
+++ b/data-raw/sites_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Itineris\ITINERIS-EVsVRE\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paolo/Files/sviluppo/R/CNR/IREA/ITINERIS.EVsVRE/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDD2688-080E-4004-B365-BD4576497937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32FCDB5-FB09-344B-9306-2BD9EE30B79A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LTER_sites" sheetId="1" r:id="rId1"/>
@@ -18,22 +18,11 @@
     <sheet name="datasets" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="184">
   <si>
     <t>https://deims.org/f30007c4-8a6e-4f11-ab87-569db54638fe</t>
   </si>
@@ -716,6 +705,15 @@
   <si>
     <t>EEA</t>
   </si>
+  <si>
+    <t xml:space="preserve">Collelongo-Selva Piana </t>
+  </si>
+  <si>
+    <t>https://deims.org/9b1d144a-dc37-4b0e-8cda-1dda1d7667da</t>
+  </si>
+  <si>
+    <t>collelongo</t>
+  </si>
 </sst>
 </file>
 
@@ -809,7 +807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -829,10 +827,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -848,7 +847,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1168,21 +1167,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="33.33203125" customWidth="1"/>
     <col min="6" max="6" width="48.6640625" customWidth="1"/>
     <col min="7" max="7" width="58.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1205,7 +1204,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1229,7 +1228,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1250,6 +1249,30 @@
       </c>
       <c r="G3" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="6" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G4" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1270,13 +1293,13 @@
       <selection activeCell="B5" activeCellId="1" sqref="B2 B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1299,7 +1322,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
@@ -1322,7 +1345,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1345,7 +1368,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -1368,7 +1391,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>62</v>
       </c>
@@ -1388,7 +1411,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>63</v>
       </c>
@@ -1411,7 +1434,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -1434,7 +1457,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>64</v>
       </c>
@@ -1457,7 +1480,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>65</v>
       </c>
@@ -1480,7 +1503,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>66</v>
       </c>
@@ -1503,7 +1526,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>67</v>
       </c>
@@ -1523,7 +1546,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>51</v>
       </c>
@@ -1546,7 +1569,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>56</v>
       </c>
@@ -1569,7 +1592,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="18.600000000000001" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>68</v>
       </c>
@@ -1616,26 +1639,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77B816B-8EFB-A44F-8A3F-6C6CC0FEF266}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="95.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="57.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="86.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="116.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="143.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="116.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="143.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="152.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="152.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -1670,7 +1693,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1700,7 +1723,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1734,7 +1757,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1767,7 +1790,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>108</v>
       </c>
@@ -1800,7 +1823,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>108</v>
       </c>
@@ -1833,7 +1856,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -1866,7 +1889,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -1899,7 +1922,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -1932,7 +1955,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -1965,7 +1988,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>108</v>
       </c>
@@ -1998,7 +2021,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>129</v>
       </c>
@@ -2031,7 +2054,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>129</v>
       </c>
@@ -2064,7 +2087,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>129</v>
       </c>
@@ -2097,7 +2120,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>129</v>
       </c>
@@ -2130,7 +2153,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>129</v>
       </c>
@@ -2163,7 +2186,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -2196,7 +2219,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>129</v>
       </c>
@@ -2229,7 +2252,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -2262,7 +2285,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>129</v>
       </c>
@@ -2295,7 +2318,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>129</v>
       </c>
@@ -2328,7 +2351,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -2361,7 +2384,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -2394,7 +2417,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -2427,7 +2450,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>129</v>
       </c>
@@ -2460,7 +2483,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>129</v>
       </c>
@@ -2493,7 +2516,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -2526,7 +2549,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>129</v>
       </c>

</xml_diff>

<commit_message>
Fix VREFolder folder name
</commit_message>
<xml_diff>
--- a/data-raw/sites_list.xlsx
+++ b/data-raw/sites_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paolo/Files/sviluppo/R/CNR/IREA/ITINERIS.EVsVRE/_Paolo_noGIT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paolo/Files/sviluppo/R/CNR/IREA/ITINERIS.EVsVRE/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{040CEFF4-E44D-0746-827F-4B6C5AECCF2D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03A4FE3-6618-E54C-97A3-24C19720D8FE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="13900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,17 +21,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">datasets!$A$1:$W$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -2006,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77B816B-8EFB-A44F-8A3F-6C6CC0FEF266}">
   <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2132,8 +2121,8 @@
         <v>88</v>
       </c>
       <c r="I2" s="8" t="str">
-        <f>+_xlfn.CONCAT("~/VRE Folders/ITINERIS_EV/DATI/",H2)</f>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/E1_Chl_2022.dat</v>
+        <f>+_xlfn.CONCAT("~/VREFolders/ITINERIS_EV/DATI/",H2)</f>
+        <v>~/VREFolders/ITINERIS_EV/DATI/E1_Chl_2022.dat</v>
       </c>
       <c r="J2" t="s">
         <v>89</v>
@@ -2169,8 +2158,8 @@
         <v>91</v>
       </c>
       <c r="I3" s="8" t="str">
-        <f t="shared" ref="I3:I52" si="0">+_xlfn.CONCAT("~/VRE Folders/ITINERIS_EV/DATI/",H3)</f>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/PR_PF_6903783.csv</v>
+        <f t="shared" ref="I3:I52" si="0">+_xlfn.CONCAT("~/VREFolders/ITINERIS_EV/DATI/",H3)</f>
+        <v>~/VREFolders/ITINERIS_EV/DATI/PR_PF_6903783.csv</v>
       </c>
       <c r="J3" t="s">
         <v>99</v>
@@ -2208,7 +2197,7 @@
       <c r="G4" s="11"/>
       <c r="I4" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/</v>
       </c>
       <c r="J4" t="s">
         <v>103</v>
@@ -2253,7 +2242,7 @@
       </c>
       <c r="I5" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/EOBS_tg_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/EOBS_tg_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J5" t="s">
         <v>137</v>
@@ -2322,7 +2311,7 @@
       </c>
       <c r="I6" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/EOBS_tn_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/EOBS_tn_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J6" t="s">
         <v>137</v>
@@ -2391,7 +2380,7 @@
       </c>
       <c r="I7" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/EOBS_tx_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/EOBS_tx_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J7" t="s">
         <v>137</v>
@@ -2460,7 +2449,7 @@
       </c>
       <c r="I8" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/EOBS_rr_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/EOBS_rr_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J8" t="s">
         <v>137</v>
@@ -2529,7 +2518,7 @@
       </c>
       <c r="I9" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/EOBS_hu_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/EOBS_hu_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J9" t="s">
         <v>137</v>
@@ -2598,7 +2587,7 @@
       </c>
       <c r="I10" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/CLC2018_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.geojson</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/CLC2018_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.geojson</v>
       </c>
       <c r="J10" t="s">
         <v>138</v>
@@ -2664,7 +2653,7 @@
       </c>
       <c r="I11" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/EEA_NPP_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/EEA_NPP_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J11" t="s">
         <v>137</v>
@@ -2728,9 +2717,9 @@
       <c r="H12" t="s">
         <v>120</v>
       </c>
-      <c r="I12" t="str">
+      <c r="I12" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_initiationts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_initiationts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J12" t="s">
         <v>137</v>
@@ -2796,7 +2785,7 @@
       </c>
       <c r="I13" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_terminationts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_terminationts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J13" t="s">
         <v>137</v>
@@ -2862,7 +2851,7 @@
       </c>
       <c r="I14" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_durationts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_durationts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J14" t="s">
         <v>137</v>
@@ -2926,9 +2915,9 @@
       <c r="H15" t="s">
         <v>123</v>
       </c>
-      <c r="I15" t="str">
+      <c r="I15" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_intchlts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_intchlts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J15" t="s">
         <v>137</v>
@@ -2994,7 +2983,7 @@
       </c>
       <c r="I16" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_meanchlts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_meanchlts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J16" t="s">
         <v>137</v>
@@ -3060,7 +3049,7 @@
       </c>
       <c r="I17" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_initiationcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_initiationcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J17" t="s">
         <v>137</v>
@@ -3124,9 +3113,9 @@
       <c r="H18" t="s">
         <v>126</v>
       </c>
-      <c r="I18" t="str">
+      <c r="I18" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_terminationcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_terminationcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J18" t="s">
         <v>137</v>
@@ -3192,7 +3181,7 @@
       </c>
       <c r="I19" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_durationcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_durationcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J19" t="s">
         <v>137</v>
@@ -3258,7 +3247,7 @@
       </c>
       <c r="I20" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_intchlcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_intchlcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J20" t="s">
         <v>137</v>
@@ -3322,9 +3311,9 @@
       <c r="H21" t="s">
         <v>129</v>
       </c>
-      <c r="I21" t="str">
+      <c r="I21" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_meanchlcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_meanchlcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J21" t="s">
         <v>137</v>
@@ -3390,7 +3379,7 @@
       </c>
       <c r="I22" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_initiationrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_initiationrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J22" t="s">
         <v>137</v>
@@ -3456,7 +3445,7 @@
       </c>
       <c r="I23" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_terminationrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_terminationrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J23" t="s">
         <v>137</v>
@@ -3520,9 +3509,9 @@
       <c r="H24" t="s">
         <v>132</v>
       </c>
-      <c r="I24" t="str">
+      <c r="I24" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_durationrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_durationrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J24" t="s">
         <v>137</v>
@@ -3588,7 +3577,7 @@
       </c>
       <c r="I25" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_intchlrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_intchlrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J25" t="s">
         <v>137</v>
@@ -3654,7 +3643,7 @@
       </c>
       <c r="I26" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_meanchlrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_meanchlrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J26" t="s">
         <v>137</v>
@@ -3718,9 +3707,9 @@
       <c r="H27" t="s">
         <v>135</v>
       </c>
-      <c r="I27" t="str">
+      <c r="I27" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_maxchl_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_maxchl_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J27" t="s">
         <v>137</v>
@@ -3786,7 +3775,7 @@
       </c>
       <c r="I28" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/Nich_maxtime_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_maxtime_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J28" t="s">
         <v>137</v>
@@ -3852,7 +3841,7 @@
       </c>
       <c r="I29" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_phyc_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_phyc_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J29" t="s">
         <v>137</v>
@@ -3919,9 +3908,9 @@
       <c r="H30" t="s">
         <v>193</v>
       </c>
-      <c r="I30" t="str">
+      <c r="I30" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_diatoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_diatoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J30" t="s">
         <v>137</v>
@@ -3990,7 +3979,7 @@
       </c>
       <c r="I31" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_nanoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_nanoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J31" t="s">
         <v>137</v>
@@ -4059,7 +4048,7 @@
       </c>
       <c r="I32" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_picoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_picoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J32" t="s">
         <v>137</v>
@@ -4126,9 +4115,9 @@
       <c r="H33" t="s">
         <v>191</v>
       </c>
-      <c r="I33" t="str">
+      <c r="I33" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_dinoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_dinoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J33" t="s">
         <v>137</v>
@@ -4197,7 +4186,7 @@
       </c>
       <c r="I34" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_chl_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_chl_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J34" t="s">
         <v>137</v>
@@ -4266,7 +4255,7 @@
       </c>
       <c r="I35" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_zooc_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_zooc_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J35" t="s">
         <v>137</v>
@@ -4333,9 +4322,9 @@
       <c r="H36" t="s">
         <v>196</v>
       </c>
-      <c r="I36" t="str">
+      <c r="I36" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_diatoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_diatoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J36" t="s">
         <v>137</v>
@@ -4404,7 +4393,7 @@
       </c>
       <c r="I37" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_nanoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_nanoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J37" t="s">
         <v>137</v>
@@ -4473,7 +4462,7 @@
       </c>
       <c r="I38" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_picoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_picoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J38" t="s">
         <v>137</v>
@@ -4540,9 +4529,9 @@
       <c r="H39" t="s">
         <v>199</v>
       </c>
-      <c r="I39" t="str">
+      <c r="I39" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_dinoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_dinoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J39" t="s">
         <v>137</v>
@@ -4611,7 +4600,7 @@
       </c>
       <c r="I40" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_o2_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_o2_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J40" t="s">
         <v>137</v>
@@ -4680,7 +4669,7 @@
       </c>
       <c r="I41" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_nppv_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_nppv_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J41" t="s">
         <v>137</v>
@@ -4749,7 +4738,7 @@
       </c>
       <c r="I42" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_nh4_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_nh4_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J42" t="s">
         <v>137</v>
@@ -4818,7 +4807,7 @@
       </c>
       <c r="I43" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_no3_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_no3_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J43" t="s">
         <v>137</v>
@@ -4887,7 +4876,7 @@
       </c>
       <c r="I44" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_po4_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_po4_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J44" t="s">
         <v>137</v>
@@ -4956,7 +4945,7 @@
       </c>
       <c r="I45" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/MedBFM4_si_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_si_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J45" t="s">
         <v>137</v>
@@ -5023,9 +5012,9 @@
       <c r="H46" t="s">
         <v>272</v>
       </c>
-      <c r="I46" t="str">
+      <c r="I46" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/CLM_AMPL_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_AMPL_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J46" t="s">
         <v>137</v>
@@ -5070,7 +5059,7 @@
       </c>
       <c r="I47" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/CLM_EOSD_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_EOSD_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J47" t="s">
         <v>137</v>
@@ -5115,7 +5104,7 @@
       </c>
       <c r="I48" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/CLM_LENGTH_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_LENGTH_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J48" t="s">
         <v>137</v>
@@ -5155,9 +5144,9 @@
       <c r="H49" t="s">
         <v>275</v>
       </c>
-      <c r="I49" t="str">
+      <c r="I49" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/CLM_LSLOPE_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_LSLOPE_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J49" t="s">
         <v>137</v>
@@ -5202,7 +5191,7 @@
       </c>
       <c r="I50" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/CLM_MAXD_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_MAXD_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J50" t="s">
         <v>137</v>
@@ -5244,7 +5233,7 @@
       </c>
       <c r="I51" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/CLM_RSLOPE_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_RSLOPE_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J51" t="s">
         <v>137</v>
@@ -5287,9 +5276,9 @@
       <c r="H52" t="s">
         <v>278</v>
       </c>
-      <c r="I52" t="str">
+      <c r="I52" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VRE Folders/ITINERIS_EV/DATI/CLM_SOSD_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_SOSD_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J52" t="s">
         <v>137</v>

</xml_diff>

<commit_message>
Fix dataset path on VRE
</commit_message>
<xml_diff>
--- a/data-raw/sites_list.xlsx
+++ b/data-raw/sites_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paolo/Files/sviluppo/R/CNR/IREA/ITINERIS.EVsVRE/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03A4FE3-6618-E54C-97A3-24C19720D8FE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E10D28-AB30-034F-879D-89747A7A6E82}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="13900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1996,7 +1996,7 @@
   <dimension ref="A1:W52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="I2" sqref="I2:I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2121,8 +2121,8 @@
         <v>88</v>
       </c>
       <c r="I2" s="8" t="str">
-        <f>+_xlfn.CONCAT("~/VREFolders/ITINERIS_EV/DATI/",H2)</f>
-        <v>~/VREFolders/ITINERIS_EV/DATI/E1_Chl_2022.dat</v>
+        <f>+_xlfn.CONCAT("~/workspace/VREFolders/ITINERIS_EV/DATI/",H2)</f>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/E1_Chl_2022.dat</v>
       </c>
       <c r="J2" t="s">
         <v>89</v>
@@ -2158,8 +2158,8 @@
         <v>91</v>
       </c>
       <c r="I3" s="8" t="str">
-        <f t="shared" ref="I3:I52" si="0">+_xlfn.CONCAT("~/VREFolders/ITINERIS_EV/DATI/",H3)</f>
-        <v>~/VREFolders/ITINERIS_EV/DATI/PR_PF_6903783.csv</v>
+        <f t="shared" ref="I3:I52" si="0">+_xlfn.CONCAT("~/workspace/VREFolders/ITINERIS_EV/DATI/",H3)</f>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/PR_PF_6903783.csv</v>
       </c>
       <c r="J3" t="s">
         <v>99</v>
@@ -2197,7 +2197,7 @@
       <c r="G4" s="11"/>
       <c r="I4" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/</v>
       </c>
       <c r="J4" t="s">
         <v>103</v>
@@ -2242,7 +2242,7 @@
       </c>
       <c r="I5" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/EOBS_tg_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/EOBS_tg_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J5" t="s">
         <v>137</v>
@@ -2311,7 +2311,7 @@
       </c>
       <c r="I6" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/EOBS_tn_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/EOBS_tn_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J6" t="s">
         <v>137</v>
@@ -2380,7 +2380,7 @@
       </c>
       <c r="I7" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/EOBS_tx_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/EOBS_tx_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J7" t="s">
         <v>137</v>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="I8" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/EOBS_rr_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/EOBS_rr_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J8" t="s">
         <v>137</v>
@@ -2518,7 +2518,7 @@
       </c>
       <c r="I9" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/EOBS_hu_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/EOBS_hu_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J9" t="s">
         <v>137</v>
@@ -2587,7 +2587,7 @@
       </c>
       <c r="I10" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/CLC2018_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.geojson</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/CLC2018_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.geojson</v>
       </c>
       <c r="J10" t="s">
         <v>138</v>
@@ -2653,7 +2653,7 @@
       </c>
       <c r="I11" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/EEA_NPP_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/EEA_NPP_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J11" t="s">
         <v>137</v>
@@ -2719,7 +2719,7 @@
       </c>
       <c r="I12" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_initiationts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_initiationts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J12" t="s">
         <v>137</v>
@@ -2785,7 +2785,7 @@
       </c>
       <c r="I13" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_terminationts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_terminationts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J13" t="s">
         <v>137</v>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="I14" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_durationts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_durationts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J14" t="s">
         <v>137</v>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="I15" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_intchlts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_intchlts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J15" t="s">
         <v>137</v>
@@ -2983,7 +2983,7 @@
       </c>
       <c r="I16" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_meanchlts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_meanchlts_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J16" t="s">
         <v>137</v>
@@ -3049,7 +3049,7 @@
       </c>
       <c r="I17" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_initiationcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_initiationcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J17" t="s">
         <v>137</v>
@@ -3115,7 +3115,7 @@
       </c>
       <c r="I18" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_terminationcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_terminationcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J18" t="s">
         <v>137</v>
@@ -3181,7 +3181,7 @@
       </c>
       <c r="I19" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_durationcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_durationcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J19" t="s">
         <v>137</v>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="I20" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_intchlcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_intchlcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J20" t="s">
         <v>137</v>
@@ -3313,7 +3313,7 @@
       </c>
       <c r="I21" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_meanchlcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_meanchlcs_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J21" t="s">
         <v>137</v>
@@ -3379,7 +3379,7 @@
       </c>
       <c r="I22" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_initiationrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_initiationrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J22" t="s">
         <v>137</v>
@@ -3445,7 +3445,7 @@
       </c>
       <c r="I23" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_terminationrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_terminationrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J23" t="s">
         <v>137</v>
@@ -3511,7 +3511,7 @@
       </c>
       <c r="I24" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_durationrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_durationrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J24" t="s">
         <v>137</v>
@@ -3577,7 +3577,7 @@
       </c>
       <c r="I25" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_intchlrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_intchlrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J25" t="s">
         <v>137</v>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="I26" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_meanchlrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_meanchlrc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J26" t="s">
         <v>137</v>
@@ -3709,7 +3709,7 @@
       </c>
       <c r="I27" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_maxchl_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_maxchl_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J27" t="s">
         <v>137</v>
@@ -3775,7 +3775,7 @@
       </c>
       <c r="I28" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/Nich_maxtime_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/Nich_maxtime_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J28" t="s">
         <v>137</v>
@@ -3841,7 +3841,7 @@
       </c>
       <c r="I29" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_phyc_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_phyc_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J29" t="s">
         <v>137</v>
@@ -3910,7 +3910,7 @@
       </c>
       <c r="I30" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_diatoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_diatoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J30" t="s">
         <v>137</v>
@@ -3979,7 +3979,7 @@
       </c>
       <c r="I31" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_nanoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_nanoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J31" t="s">
         <v>137</v>
@@ -4048,7 +4048,7 @@
       </c>
       <c r="I32" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_picoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_picoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J32" t="s">
         <v>137</v>
@@ -4117,7 +4117,7 @@
       </c>
       <c r="I33" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_dinoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_dinoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J33" t="s">
         <v>137</v>
@@ -4186,7 +4186,7 @@
       </c>
       <c r="I34" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_chl_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_chl_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J34" t="s">
         <v>137</v>
@@ -4255,7 +4255,7 @@
       </c>
       <c r="I35" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_zooc_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_zooc_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J35" t="s">
         <v>137</v>
@@ -4324,7 +4324,7 @@
       </c>
       <c r="I36" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_diatoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_diatoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J36" t="s">
         <v>137</v>
@@ -4393,7 +4393,7 @@
       </c>
       <c r="I37" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_nanoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_nanoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J37" t="s">
         <v>137</v>
@@ -4462,7 +4462,7 @@
       </c>
       <c r="I38" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_picoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_picoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J38" t="s">
         <v>137</v>
@@ -4531,7 +4531,7 @@
       </c>
       <c r="I39" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_dinoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_dinoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J39" t="s">
         <v>137</v>
@@ -4600,7 +4600,7 @@
       </c>
       <c r="I40" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_o2_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_o2_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J40" t="s">
         <v>137</v>
@@ -4669,7 +4669,7 @@
       </c>
       <c r="I41" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_nppv_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_nppv_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J41" t="s">
         <v>137</v>
@@ -4738,7 +4738,7 @@
       </c>
       <c r="I42" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_nh4_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_nh4_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J42" t="s">
         <v>137</v>
@@ -4807,7 +4807,7 @@
       </c>
       <c r="I43" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_no3_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_no3_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J43" t="s">
         <v>137</v>
@@ -4876,7 +4876,7 @@
       </c>
       <c r="I44" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_po4_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_po4_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J44" t="s">
         <v>137</v>
@@ -4945,7 +4945,7 @@
       </c>
       <c r="I45" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/MedBFM4_si_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_si_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
       </c>
       <c r="J45" t="s">
         <v>137</v>
@@ -5014,7 +5014,7 @@
       </c>
       <c r="I46" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_AMPL_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/CLM_AMPL_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J46" t="s">
         <v>137</v>
@@ -5059,7 +5059,7 @@
       </c>
       <c r="I47" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_EOSD_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/CLM_EOSD_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J47" t="s">
         <v>137</v>
@@ -5104,7 +5104,7 @@
       </c>
       <c r="I48" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_LENGTH_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/CLM_LENGTH_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J48" t="s">
         <v>137</v>
@@ -5146,7 +5146,7 @@
       </c>
       <c r="I49" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_LSLOPE_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/CLM_LSLOPE_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J49" t="s">
         <v>137</v>
@@ -5191,7 +5191,7 @@
       </c>
       <c r="I50" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_MAXD_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/CLM_MAXD_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J50" t="s">
         <v>137</v>
@@ -5233,7 +5233,7 @@
       </c>
       <c r="I51" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_RSLOPE_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/CLM_RSLOPE_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J51" t="s">
         <v>137</v>
@@ -5278,7 +5278,7 @@
       </c>
       <c r="I52" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/VREFolders/ITINERIS_EV/DATI/CLM_SOSD_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/CLM_SOSD_9b1d144a-dc37-4b0e-8cda-1dda1d7667da.tif</v>
       </c>
       <c r="J52" t="s">
         <v>137</v>

</xml_diff>

<commit_message>
Fix spaces in dataset filenames
</commit_message>
<xml_diff>
--- a/data-raw/sites_list.xlsx
+++ b/data-raw/sites_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paolo/Files/sviluppo/R/CNR/IREA/ITINERIS.EVsVRE/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E10D28-AB30-034F-879D-89747A7A6E82}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB67A534-345C-4C4D-A704-7C9057B9C59D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="13900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -733,45 +733,6 @@
     <t>https://deims.org/9b1d144a-dc37-4b0e-8cda-1dda1d7667da</t>
   </si>
   <si>
-    <t>MedBFM4_nanoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_picoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_dinoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_phyc_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_diatoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_chl_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_zooc_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_diatoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_nanoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_picoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_dinoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_o2_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_nppv_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
     <t>Monthly concentration of ammonium in sea water (2022-2024) Delta Po - Costa Romagnola</t>
   </si>
   <si>
@@ -784,18 +745,6 @@
     <t>Monthly concentration of silicates in sea water (2022-2024) Delta Po - Costa Romagnola</t>
   </si>
   <si>
-    <t>MedBFM4_nh4_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_no3_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_po4_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
-    <t>MedBFM4_si_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</t>
-  </si>
-  <si>
     <t>Var_identifier</t>
   </si>
   <si>
@@ -1058,6 +1007,57 @@
   </si>
   <si>
     <t>surface_precipitation</t>
+  </si>
+  <si>
+    <t>MedBFM4_si_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_phyc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_diatoC_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_nanoC_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_picoC_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_dinoC_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_chl_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_zooc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_diatoChla_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_nanoChla_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_picoChla_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_dinoChla_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_o2_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_nppv_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_nh4_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_no3_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
+  </si>
+  <si>
+    <t>MedBFM4_po4_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</t>
   </si>
 </sst>
 </file>
@@ -1995,8 +1995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77B816B-8EFB-A44F-8A3F-6C6CC0FEF266}">
   <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I52"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2028,7 +2028,7 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="B1" t="s">
         <v>80</v>
@@ -2040,13 +2040,13 @@
         <v>93</v>
       </c>
       <c r="E1" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="F1" t="s">
         <v>85</v>
       </c>
       <c r="G1" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
       <c r="H1" t="s">
         <v>87</v>
@@ -2061,13 +2061,13 @@
         <v>8</v>
       </c>
       <c r="L1" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="M1" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
       <c r="N1" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="O1" t="s">
         <v>95</v>
@@ -2076,25 +2076,25 @@
         <v>98</v>
       </c>
       <c r="Q1" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="R1" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="S1" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="T1" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="U1" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="V1" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="W1" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -2111,7 +2111,7 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F2" t="s">
         <v>90</v>
@@ -2148,7 +2148,7 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F3" t="s">
         <v>92</v>
@@ -2189,7 +2189,7 @@
         <v>59</v>
       </c>
       <c r="E4" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="F4" t="s">
         <v>102</v>
@@ -2229,13 +2229,13 @@
         <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="F5" t="s">
         <v>107</v>
       </c>
       <c r="G5" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="H5" t="s">
         <v>118</v>
@@ -2254,34 +2254,34 @@
         <v>166</v>
       </c>
       <c r="N5" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O5" t="s">
         <v>169</v>
       </c>
       <c r="P5" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q5" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="R5">
         <v>0.1</v>
       </c>
       <c r="S5" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T5" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="U5" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="V5" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W5" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:23">
@@ -2298,13 +2298,13 @@
         <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="F6" t="s">
         <v>108</v>
       </c>
       <c r="G6" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="H6" t="s">
         <v>117</v>
@@ -2323,34 +2323,34 @@
         <v>166</v>
       </c>
       <c r="N6" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O6" t="s">
         <v>169</v>
       </c>
       <c r="P6" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q6" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="R6">
         <v>0.1</v>
       </c>
       <c r="S6" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T6" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="U6" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="V6" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W6" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:23">
@@ -2367,13 +2367,13 @@
         <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="F7" t="s">
         <v>109</v>
       </c>
       <c r="G7" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="H7" t="s">
         <v>116</v>
@@ -2392,34 +2392,34 @@
         <v>166</v>
       </c>
       <c r="N7" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O7" t="s">
         <v>169</v>
       </c>
       <c r="P7" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q7" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="R7">
         <v>0.1</v>
       </c>
       <c r="S7" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T7" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="U7" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="V7" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W7" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:23">
@@ -2436,13 +2436,13 @@
         <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="F8" t="s">
         <v>110</v>
       </c>
       <c r="G8" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="H8" t="s">
         <v>115</v>
@@ -2461,34 +2461,34 @@
         <v>166</v>
       </c>
       <c r="N8" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O8" t="s">
         <v>169</v>
       </c>
       <c r="P8" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q8" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="R8">
         <v>0.1</v>
       </c>
       <c r="S8" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T8" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="U8" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="V8" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W8" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:23">
@@ -2505,13 +2505,13 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="F9" t="s">
         <v>111</v>
       </c>
       <c r="G9" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="H9" t="s">
         <v>114</v>
@@ -2530,34 +2530,34 @@
         <v>166</v>
       </c>
       <c r="N9" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="O9" t="s">
         <v>169</v>
       </c>
       <c r="P9" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q9" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="R9">
         <v>0.1</v>
       </c>
       <c r="S9" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T9" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="U9" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="V9" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W9" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:23">
@@ -2571,16 +2571,16 @@
         <v>66</v>
       </c>
       <c r="D10" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="E10" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="F10" t="s">
         <v>112</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="H10" t="s">
         <v>113</v>
@@ -2602,28 +2602,28 @@
         <v>169</v>
       </c>
       <c r="P10" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q10" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="R10">
         <v>25</v>
       </c>
       <c r="S10" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="T10" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="U10" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="V10" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W10" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:23">
@@ -2640,16 +2640,16 @@
         <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="F11" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="G11" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="H11" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="I11" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2668,10 +2668,10 @@
         <v>170</v>
       </c>
       <c r="P11" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="Q11" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R11">
         <v>196</v>
@@ -2680,16 +2680,16 @@
         <v>76</v>
       </c>
       <c r="T11" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U11" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="V11" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W11" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:23">
@@ -2706,13 +2706,13 @@
         <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="F12" t="s">
         <v>146</v>
       </c>
       <c r="G12" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="H12" t="s">
         <v>120</v>
@@ -2731,31 +2731,31 @@
         <v>165</v>
       </c>
       <c r="N12" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O12" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R12">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U12" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V12" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W12" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:23">
@@ -2772,13 +2772,13 @@
         <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="F13" t="s">
         <v>147</v>
       </c>
       <c r="G13" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="H13" t="s">
         <v>121</v>
@@ -2797,31 +2797,31 @@
         <v>165</v>
       </c>
       <c r="N13" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O13" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R13">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S13" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U13" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V13" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W13" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:23">
@@ -2838,13 +2838,13 @@
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="F14" t="s">
         <v>148</v>
       </c>
       <c r="G14" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="H14" t="s">
         <v>122</v>
@@ -2863,31 +2863,31 @@
         <v>165</v>
       </c>
       <c r="N14" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O14" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R14">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S14" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U14" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V14" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W14" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:23">
@@ -2904,13 +2904,13 @@
         <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F15" t="s">
         <v>149</v>
       </c>
       <c r="G15" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="H15" t="s">
         <v>123</v>
@@ -2929,31 +2929,31 @@
         <v>165</v>
       </c>
       <c r="N15" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O15" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q15" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R15">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S15" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U15" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V15" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W15" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:23">
@@ -2970,13 +2970,13 @@
         <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F16" t="s">
         <v>150</v>
       </c>
       <c r="G16" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="H16" t="s">
         <v>124</v>
@@ -2995,31 +2995,31 @@
         <v>165</v>
       </c>
       <c r="N16" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O16" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R16">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S16" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T16" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U16" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V16" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W16" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:23">
@@ -3036,13 +3036,13 @@
         <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="F17" t="s">
         <v>151</v>
       </c>
       <c r="G17" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="H17" t="s">
         <v>125</v>
@@ -3061,31 +3061,31 @@
         <v>165</v>
       </c>
       <c r="N17" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O17" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q17" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R17">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S17" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T17" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U17" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V17" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W17" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:23">
@@ -3102,13 +3102,13 @@
         <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="F18" t="s">
         <v>152</v>
       </c>
       <c r="G18" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="H18" t="s">
         <v>126</v>
@@ -3127,31 +3127,31 @@
         <v>165</v>
       </c>
       <c r="N18" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O18" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q18" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R18">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S18" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U18" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V18" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W18" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:23">
@@ -3168,13 +3168,13 @@
         <v>26</v>
       </c>
       <c r="E19" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="F19" t="s">
         <v>153</v>
       </c>
       <c r="G19" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="H19" t="s">
         <v>127</v>
@@ -3193,31 +3193,31 @@
         <v>165</v>
       </c>
       <c r="N19" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O19" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q19" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R19">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S19" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T19" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U19" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V19" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W19" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:23">
@@ -3234,13 +3234,13 @@
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F20" t="s">
         <v>154</v>
       </c>
       <c r="G20" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="H20" t="s">
         <v>128</v>
@@ -3259,31 +3259,31 @@
         <v>165</v>
       </c>
       <c r="N20" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O20" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q20" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R20">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S20" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T20" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U20" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V20" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W20" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:23">
@@ -3300,13 +3300,13 @@
         <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F21" t="s">
         <v>155</v>
       </c>
       <c r="G21" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="H21" t="s">
         <v>129</v>
@@ -3325,31 +3325,31 @@
         <v>165</v>
       </c>
       <c r="N21" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O21" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q21" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R21">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S21" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T21" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U21" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V21" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W21" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:23">
@@ -3366,13 +3366,13 @@
         <v>26</v>
       </c>
       <c r="E22" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="F22" t="s">
         <v>156</v>
       </c>
       <c r="G22" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="H22" t="s">
         <v>130</v>
@@ -3391,31 +3391,31 @@
         <v>165</v>
       </c>
       <c r="N22" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O22" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q22" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R22">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S22" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U22" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V22" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W22" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:23">
@@ -3432,13 +3432,13 @@
         <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="F23" t="s">
         <v>157</v>
       </c>
       <c r="G23" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="H23" t="s">
         <v>131</v>
@@ -3457,31 +3457,31 @@
         <v>165</v>
       </c>
       <c r="N23" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O23" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q23" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R23">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S23" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T23" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U23" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V23" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W23" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:23">
@@ -3498,13 +3498,13 @@
         <v>26</v>
       </c>
       <c r="E24" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="F24" t="s">
         <v>158</v>
       </c>
       <c r="G24" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="H24" t="s">
         <v>132</v>
@@ -3523,31 +3523,31 @@
         <v>165</v>
       </c>
       <c r="N24" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O24" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q24" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R24">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S24" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T24" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U24" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V24" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W24" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -3564,13 +3564,13 @@
         <v>19</v>
       </c>
       <c r="E25" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F25" t="s">
         <v>159</v>
       </c>
       <c r="G25" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="H25" t="s">
         <v>133</v>
@@ -3589,31 +3589,31 @@
         <v>165</v>
       </c>
       <c r="N25" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O25" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q25" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R25">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S25" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T25" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U25" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V25" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W25" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:23">
@@ -3630,13 +3630,13 @@
         <v>19</v>
       </c>
       <c r="E26" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F26" t="s">
         <v>160</v>
       </c>
       <c r="G26" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="H26" t="s">
         <v>134</v>
@@ -3655,31 +3655,31 @@
         <v>165</v>
       </c>
       <c r="N26" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O26" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q26" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R26">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S26" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T26" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U26" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V26" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W26" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27" spans="1:23">
@@ -3696,13 +3696,13 @@
         <v>19</v>
       </c>
       <c r="E27" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F27" t="s">
         <v>161</v>
       </c>
       <c r="G27" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="H27" t="s">
         <v>135</v>
@@ -3721,31 +3721,31 @@
         <v>165</v>
       </c>
       <c r="N27" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O27" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q27" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R27">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S27" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T27" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U27" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V27" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W27" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:23">
@@ -3762,13 +3762,13 @@
         <v>19</v>
       </c>
       <c r="E28" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F28" t="s">
         <v>162</v>
       </c>
       <c r="G28" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
       <c r="H28" t="s">
         <v>136</v>
@@ -3787,31 +3787,31 @@
         <v>165</v>
       </c>
       <c r="N28" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="O28" s="11" t="s">
         <v>139</v>
       </c>
       <c r="Q28" s="12" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="R28">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S28" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T28" s="12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="U28" s="12" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="V28" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W28" s="12" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:23">
@@ -3828,59 +3828,59 @@
         <v>30</v>
       </c>
       <c r="E29" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="F29" t="s">
         <v>171</v>
       </c>
       <c r="G29" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="H29" t="s">
-        <v>192</v>
+        <v>282</v>
       </c>
       <c r="I29" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_phyc_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_phyc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J29" t="s">
         <v>137</v>
       </c>
       <c r="K29" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="M29" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N29" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="O29" t="s">
         <v>169</v>
       </c>
       <c r="P29" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q29" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R29">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S29" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T29" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U29" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V29" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W29" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:23">
@@ -3897,59 +3897,59 @@
         <v>30</v>
       </c>
       <c r="E30" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="F30" t="s">
         <v>172</v>
       </c>
       <c r="G30" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="H30" t="s">
-        <v>193</v>
+        <v>283</v>
       </c>
       <c r="I30" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_diatoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_diatoC_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J30" t="s">
         <v>137</v>
       </c>
       <c r="K30" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="M30" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N30" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="O30" t="s">
         <v>169</v>
       </c>
       <c r="P30" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q30" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R30">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S30" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T30" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U30" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V30" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W30" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:23">
@@ -3966,59 +3966,59 @@
         <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="F31" t="s">
         <v>173</v>
       </c>
       <c r="G31" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="H31" t="s">
-        <v>189</v>
+        <v>284</v>
       </c>
       <c r="I31" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_nanoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_nanoC_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J31" t="s">
         <v>137</v>
       </c>
       <c r="K31" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="M31" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N31" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="O31" t="s">
         <v>169</v>
       </c>
       <c r="P31" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q31" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R31">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S31" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T31" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U31" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V31" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W31" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="1:23">
@@ -4035,59 +4035,59 @@
         <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="F32" t="s">
         <v>174</v>
       </c>
       <c r="G32" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="H32" t="s">
-        <v>190</v>
+        <v>285</v>
       </c>
       <c r="I32" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_picoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_picoC_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J32" t="s">
         <v>137</v>
       </c>
       <c r="K32" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="M32" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N32" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="O32" t="s">
         <v>169</v>
       </c>
       <c r="P32" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q32" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R32">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S32" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T32" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U32" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V32" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W32" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:23">
@@ -4104,59 +4104,59 @@
         <v>30</v>
       </c>
       <c r="E33" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="F33" t="s">
         <v>175</v>
       </c>
       <c r="G33" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="H33" t="s">
-        <v>191</v>
+        <v>286</v>
       </c>
       <c r="I33" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_dinoC_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_dinoC_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J33" t="s">
         <v>137</v>
       </c>
       <c r="K33" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="M33" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N33" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="O33" t="s">
         <v>169</v>
       </c>
       <c r="P33" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q33" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R33">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S33" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T33" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U33" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V33" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W33" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:23">
@@ -4173,59 +4173,59 @@
         <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F34" t="s">
         <v>177</v>
       </c>
       <c r="G34" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="H34" t="s">
-        <v>194</v>
+        <v>287</v>
       </c>
       <c r="I34" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_chl_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_chl_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J34" t="s">
         <v>137</v>
       </c>
       <c r="K34" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="M34" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N34" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="O34" t="s">
         <v>169</v>
       </c>
       <c r="P34" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q34" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R34">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S34" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T34" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U34" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V34" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W34" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:23">
@@ -4242,59 +4242,59 @@
         <v>30</v>
       </c>
       <c r="E35" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="F35" t="s">
         <v>178</v>
       </c>
       <c r="G35" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="H35" t="s">
-        <v>195</v>
+        <v>288</v>
       </c>
       <c r="I35" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_zooc_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_zooc_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J35" t="s">
         <v>137</v>
       </c>
       <c r="K35" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="M35" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N35" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="O35" t="s">
         <v>169</v>
       </c>
       <c r="P35" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q35" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R35">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S35" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T35" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U35" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V35" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W35" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:23">
@@ -4311,59 +4311,59 @@
         <v>19</v>
       </c>
       <c r="E36" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F36" t="s">
         <v>179</v>
       </c>
       <c r="G36" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="H36" t="s">
-        <v>196</v>
+        <v>289</v>
       </c>
       <c r="I36" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_diatoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_diatoChla_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J36" t="s">
         <v>137</v>
       </c>
       <c r="K36" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="M36" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N36" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="O36" t="s">
         <v>169</v>
       </c>
       <c r="P36" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q36" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R36">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S36" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T36" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U36" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V36" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W36" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="37" spans="1:23">
@@ -4380,59 +4380,59 @@
         <v>19</v>
       </c>
       <c r="E37" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F37" t="s">
         <v>180</v>
       </c>
       <c r="G37" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="H37" t="s">
-        <v>197</v>
+        <v>290</v>
       </c>
       <c r="I37" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_nanoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_nanoChla_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J37" t="s">
         <v>137</v>
       </c>
       <c r="K37" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="M37" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N37" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="O37" t="s">
         <v>169</v>
       </c>
       <c r="P37" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q37" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R37">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S37" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T37" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U37" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V37" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W37" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="1:23">
@@ -4449,59 +4449,59 @@
         <v>19</v>
       </c>
       <c r="E38" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F38" t="s">
         <v>181</v>
       </c>
       <c r="G38" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="H38" t="s">
-        <v>198</v>
+        <v>291</v>
       </c>
       <c r="I38" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_picoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_picoChla_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J38" t="s">
         <v>137</v>
       </c>
       <c r="K38" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="M38" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N38" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="O38" t="s">
         <v>169</v>
       </c>
       <c r="P38" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q38" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R38">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S38" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T38" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U38" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V38" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W38" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:23">
@@ -4518,59 +4518,59 @@
         <v>19</v>
       </c>
       <c r="E39" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="F39" t="s">
         <v>182</v>
       </c>
       <c r="G39" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
       <c r="H39" t="s">
-        <v>199</v>
+        <v>292</v>
       </c>
       <c r="I39" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_dinoChla_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_dinoChla_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J39" t="s">
         <v>137</v>
       </c>
       <c r="K39" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="M39" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N39" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="O39" t="s">
         <v>169</v>
       </c>
       <c r="P39" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q39" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R39">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S39" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T39" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U39" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V39" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W39" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:23">
@@ -4587,59 +4587,59 @@
         <v>23</v>
       </c>
       <c r="E40" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="F40" t="s">
         <v>184</v>
       </c>
       <c r="G40" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="H40" t="s">
-        <v>200</v>
+        <v>293</v>
       </c>
       <c r="I40" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_o2_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_o2_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J40" t="s">
         <v>137</v>
       </c>
       <c r="K40" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="M40" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N40" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="O40" t="s">
         <v>169</v>
       </c>
       <c r="P40" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q40" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R40">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S40" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T40" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U40" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V40" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W40" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="41" spans="1:23">
@@ -4656,59 +4656,59 @@
         <v>30</v>
       </c>
       <c r="E41" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="F41" t="s">
         <v>185</v>
       </c>
       <c r="G41" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="H41" t="s">
-        <v>201</v>
+        <v>294</v>
       </c>
       <c r="I41" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_nppv_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_nppv_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J41" t="s">
         <v>137</v>
       </c>
       <c r="K41" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="M41" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N41" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="O41" t="s">
         <v>169</v>
       </c>
       <c r="P41" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q41" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R41">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S41" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T41" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U41" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V41" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W41" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" spans="1:23">
@@ -4725,59 +4725,59 @@
         <v>13</v>
       </c>
       <c r="E42" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="F42" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="G42" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="H42" t="s">
-        <v>206</v>
+        <v>295</v>
       </c>
       <c r="I42" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_nh4_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_nh4_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J42" t="s">
         <v>137</v>
       </c>
       <c r="K42" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="M42" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N42" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="O42" t="s">
         <v>169</v>
       </c>
       <c r="P42" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q42" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R42">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S42" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T42" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U42" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V42" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W42" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" spans="1:23">
@@ -4794,59 +4794,59 @@
         <v>13</v>
       </c>
       <c r="E43" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="F43" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="G43" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="H43" t="s">
-        <v>207</v>
+        <v>296</v>
       </c>
       <c r="I43" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_no3_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_no3_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J43" t="s">
         <v>137</v>
       </c>
       <c r="K43" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="M43" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N43" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="O43" t="s">
         <v>169</v>
       </c>
       <c r="P43" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q43" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R43">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S43" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T43" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U43" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V43" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W43" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="44" spans="1:23">
@@ -4863,59 +4863,59 @@
         <v>13</v>
       </c>
       <c r="E44" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="F44" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="G44" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="H44" t="s">
-        <v>208</v>
+        <v>297</v>
       </c>
       <c r="I44" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_po4_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_po4_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J44" t="s">
         <v>137</v>
       </c>
       <c r="K44" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="M44" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N44" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="O44" t="s">
         <v>169</v>
       </c>
       <c r="P44" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q44" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R44">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S44" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T44" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U44" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V44" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W44" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:23">
@@ -4932,59 +4932,59 @@
         <v>13</v>
       </c>
       <c r="E45" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="F45" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="G45" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="H45" t="s">
-        <v>209</v>
+        <v>281</v>
       </c>
       <c r="I45" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_si_6869436a-80f4-4c6d-954b-a730b348d7ce .tif</v>
+        <v>~/workspace/VREFolders/ITINERIS_EV/DATI/MedBFM4_si_6869436a-80f4-4c6d-954b-a730b348d7ce.tif</v>
       </c>
       <c r="J45" t="s">
         <v>137</v>
       </c>
       <c r="K45" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="M45" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="N45" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="O45" t="s">
         <v>169</v>
       </c>
       <c r="P45" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="Q45" s="12" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="R45">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="S45" s="12" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="T45" s="12" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="U45" s="12" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="V45" s="12" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="W45" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:23">
@@ -5001,16 +5001,16 @@
         <v>48</v>
       </c>
       <c r="E46" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="F46" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="G46" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="H46" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="I46" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5020,16 +5020,16 @@
         <v>137</v>
       </c>
       <c r="M46" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="N46" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="O46" t="s">
         <v>169</v>
       </c>
       <c r="P46" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47" spans="1:23">
@@ -5046,16 +5046,16 @@
         <v>48</v>
       </c>
       <c r="E47" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="F47" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="G47" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="H47" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="I47" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5065,16 +5065,16 @@
         <v>137</v>
       </c>
       <c r="M47" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="N47" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="O47" t="s">
         <v>169</v>
       </c>
       <c r="P47" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="48" spans="1:23">
@@ -5091,16 +5091,16 @@
         <v>48</v>
       </c>
       <c r="E48" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="F48" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
       <c r="G48" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
       <c r="H48" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="I48" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5110,16 +5110,16 @@
         <v>137</v>
       </c>
       <c r="M48" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="N48" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="O48" t="s">
         <v>169</v>
       </c>
       <c r="P48" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -5136,13 +5136,13 @@
         <v>48</v>
       </c>
       <c r="E49" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="F49" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="H49" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="I49" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5152,16 +5152,16 @@
         <v>137</v>
       </c>
       <c r="M49" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="N49" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="O49" t="s">
         <v>169</v>
       </c>
       <c r="P49" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -5178,16 +5178,16 @@
         <v>48</v>
       </c>
       <c r="E50" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="F50" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="G50" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="H50" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="I50" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5197,16 +5197,16 @@
         <v>137</v>
       </c>
       <c r="M50" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
       <c r="N50" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="O50" t="s">
         <v>169</v>
       </c>
       <c r="P50" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -5223,13 +5223,13 @@
         <v>48</v>
       </c>
       <c r="E51" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="F51" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
       <c r="H51" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="I51" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5239,16 +5239,16 @@
         <v>137</v>
       </c>
       <c r="M51" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="N51" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="O51" t="s">
         <v>169</v>
       </c>
       <c r="P51" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -5265,16 +5265,16 @@
         <v>48</v>
       </c>
       <c r="E52" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="F52" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="G52" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
       <c r="H52" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="I52" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5284,16 +5284,16 @@
         <v>137</v>
       </c>
       <c r="M52" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
       <c r="N52" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="O52" t="s">
         <v>169</v>
       </c>
       <c r="P52" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Temporarly remove wrong ncfileNames to be fixed
</commit_message>
<xml_diff>
--- a/data-raw/sites_list.xlsx
+++ b/data-raw/sites_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Itineris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E68F185-CF66-40B4-BF1A-E2F57A0E3C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2ED003-A9BE-41FF-B268-D181DE21700E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="472">
   <si>
     <t>https://deims.org/f30007c4-8a6e-4f11-ab87-569db54638fe</t>
   </si>
@@ -1435,15 +1435,6 @@
   </si>
   <si>
     <t>/home/jovyan/itineris-dataspace/VRE_EV/DATI/Nich_6869436a-80f4-4c6d-954b-a730b348d7ce_cut.nc</t>
-  </si>
-  <si>
-    <t>/home/jovyan/itineris-dataspace/VRE_EV/DATI/MedBFM4m_Chlorophyll_6869436a-80f4-4c6d-954b-a730b348d7ce_cut.nc</t>
-  </si>
-  <si>
-    <t>/home/jovyan/itineris-dataspace/VRE_EV/DATI/MedBFM4m_Oxygen_6869436a-80f4-4c6d-954b-a730b348d7ce_cut.nc</t>
-  </si>
-  <si>
-    <t>/home/jovyan/itineris-dataspace/VRE_EV/DATI/MedBFM4m_Nutrients_6869436a-80f4-4c6d-954b-a730b348d7ce_cut.nc</t>
   </si>
   <si>
     <t>/home/jovyan/itineris-dataspace/VRE_EV/DATI/E1_Chl_2022.dat</t>
@@ -2547,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77B816B-8EFB-A44F-8A3F-6C6CC0FEF266}">
   <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" topLeftCell="Y7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Z38" sqref="Z38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2692,7 +2683,7 @@
         <v>88</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="J2" t="s">
         <v>89</v>
@@ -2731,7 +2722,7 @@
         <v>91</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="J3" t="s">
         <v>99</v>
@@ -2776,7 +2767,7 @@
         <v>379</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="J4" t="s">
         <v>89</v>
@@ -2850,7 +2841,7 @@
         <v>115</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="J5" t="s">
         <v>134</v>
@@ -2933,7 +2924,7 @@
         <v>114</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="J6" t="s">
         <v>134</v>
@@ -3016,7 +3007,7 @@
         <v>113</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="J7" t="s">
         <v>134</v>
@@ -3099,7 +3090,7 @@
         <v>112</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="J8" t="s">
         <v>134</v>
@@ -3182,7 +3173,7 @@
         <v>111</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="J9" t="s">
         <v>134</v>
@@ -3265,7 +3256,7 @@
         <v>110</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="J10" t="s">
         <v>135</v>
@@ -3336,7 +3327,7 @@
         <v>249</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="J11" t="s">
         <v>134</v>
@@ -3407,7 +3398,7 @@
         <v>117</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J12" t="s">
         <v>339</v>
@@ -3490,7 +3481,7 @@
         <v>118</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="J13" t="s">
         <v>134</v>
@@ -3573,7 +3564,7 @@
         <v>119</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="J14" t="s">
         <v>134</v>
@@ -3656,7 +3647,7 @@
         <v>120</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="J15" t="s">
         <v>134</v>
@@ -3739,7 +3730,7 @@
         <v>121</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="J16" t="s">
         <v>134</v>
@@ -3822,7 +3813,7 @@
         <v>122</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="J17" t="s">
         <v>134</v>
@@ -3905,7 +3896,7 @@
         <v>123</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="J18" t="s">
         <v>134</v>
@@ -3988,7 +3979,7 @@
         <v>124</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="J19" t="s">
         <v>134</v>
@@ -4071,7 +4062,7 @@
         <v>125</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="J20" t="s">
         <v>134</v>
@@ -4154,7 +4145,7 @@
         <v>126</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="J21" t="s">
         <v>134</v>
@@ -4237,7 +4228,7 @@
         <v>127</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="J22" t="s">
         <v>134</v>
@@ -4320,7 +4311,7 @@
         <v>128</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="J23" t="s">
         <v>134</v>
@@ -4403,7 +4394,7 @@
         <v>129</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="J24" t="s">
         <v>134</v>
@@ -4486,7 +4477,7 @@
         <v>130</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="J25" t="s">
         <v>134</v>
@@ -4569,7 +4560,7 @@
         <v>131</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="J26" t="s">
         <v>134</v>
@@ -4652,7 +4643,7 @@
         <v>132</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="J27" t="s">
         <v>134</v>
@@ -4735,7 +4726,7 @@
         <v>133</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="J28" t="s">
         <v>134</v>
@@ -4818,7 +4809,7 @@
         <v>278</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="J29" t="s">
         <v>134</v>
@@ -4865,9 +4856,7 @@
       <c r="Y29" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="Z29" s="8" t="s">
-        <v>420</v>
-      </c>
+      <c r="Z29" s="8"/>
       <c r="AA29" s="15" t="s">
         <v>305</v>
       </c>
@@ -4901,7 +4890,7 @@
         <v>279</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="J30" t="s">
         <v>134</v>
@@ -4948,9 +4937,7 @@
       <c r="Y30" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="Z30" s="8" t="s">
-        <v>420</v>
-      </c>
+      <c r="Z30" s="8"/>
       <c r="AA30" s="15" t="s">
         <v>306</v>
       </c>
@@ -4984,7 +4971,7 @@
         <v>280</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="J31" t="s">
         <v>134</v>
@@ -5031,9 +5018,7 @@
       <c r="Y31" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="Z31" s="8" t="s">
-        <v>420</v>
-      </c>
+      <c r="Z31" s="8"/>
       <c r="AA31" s="15" t="s">
         <v>307</v>
       </c>
@@ -5067,7 +5052,7 @@
         <v>281</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="J32" t="s">
         <v>134</v>
@@ -5114,9 +5099,7 @@
       <c r="Y32" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="Z32" s="8" t="s">
-        <v>420</v>
-      </c>
+      <c r="Z32" s="8"/>
       <c r="AA32" s="15" t="s">
         <v>308</v>
       </c>
@@ -5150,7 +5133,7 @@
         <v>282</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="J33" t="s">
         <v>134</v>
@@ -5197,9 +5180,7 @@
       <c r="Y33" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="Z33" s="8" t="s">
-        <v>420</v>
-      </c>
+      <c r="Z33" s="8"/>
       <c r="AA33" s="15" t="s">
         <v>309</v>
       </c>
@@ -5233,7 +5214,7 @@
         <v>283</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="J34" t="s">
         <v>134</v>
@@ -5280,9 +5261,7 @@
       <c r="Y34" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="Z34" s="8" t="s">
-        <v>420</v>
-      </c>
+      <c r="Z34" s="8"/>
       <c r="AA34" s="15" t="s">
         <v>310</v>
       </c>
@@ -5316,7 +5295,7 @@
         <v>284</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="J35" t="s">
         <v>134</v>
@@ -5363,9 +5342,7 @@
       <c r="Y35" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="Z35" s="8" t="s">
-        <v>420</v>
-      </c>
+      <c r="Z35" s="8"/>
       <c r="AA35" s="15" t="s">
         <v>311</v>
       </c>
@@ -5399,7 +5376,7 @@
         <v>285</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="J36" t="s">
         <v>134</v>
@@ -5446,9 +5423,7 @@
       <c r="Y36" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="Z36" s="8" t="s">
-        <v>420</v>
-      </c>
+      <c r="Z36" s="8"/>
       <c r="AA36" s="15" t="s">
         <v>312</v>
       </c>
@@ -5482,7 +5457,7 @@
         <v>286</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="J37" t="s">
         <v>134</v>
@@ -5529,9 +5504,7 @@
       <c r="Y37" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="Z37" s="8" t="s">
-        <v>420</v>
-      </c>
+      <c r="Z37" s="8"/>
       <c r="AA37" s="15" t="s">
         <v>313</v>
       </c>
@@ -5565,7 +5538,7 @@
         <v>287</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="J38" t="s">
         <v>134</v>
@@ -5612,9 +5585,7 @@
       <c r="Y38" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="Z38" s="8" t="s">
-        <v>420</v>
-      </c>
+      <c r="Z38" s="8"/>
       <c r="AA38" s="15" t="s">
         <v>314</v>
       </c>
@@ -5648,7 +5619,7 @@
         <v>288</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="J39" t="s">
         <v>134</v>
@@ -5695,9 +5666,7 @@
       <c r="Y39" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="Z39" s="8" t="s">
-        <v>420</v>
-      </c>
+      <c r="Z39" s="8"/>
       <c r="AA39" s="15" t="s">
         <v>315</v>
       </c>
@@ -5731,7 +5700,7 @@
         <v>289</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="J40" t="s">
         <v>134</v>
@@ -5778,9 +5747,7 @@
       <c r="Y40" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="Z40" s="8" t="s">
-        <v>421</v>
-      </c>
+      <c r="Z40" s="8"/>
       <c r="AA40" s="15" t="s">
         <v>316</v>
       </c>
@@ -5814,7 +5781,7 @@
         <v>290</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="J41" t="s">
         <v>134</v>
@@ -5861,9 +5828,7 @@
       <c r="Y41" s="8" t="s">
         <v>341</v>
       </c>
-      <c r="Z41" s="8" t="s">
-        <v>421</v>
-      </c>
+      <c r="Z41" s="8"/>
       <c r="AA41" s="15" t="s">
         <v>317</v>
       </c>
@@ -5897,7 +5862,7 @@
         <v>291</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="J42" t="s">
         <v>134</v>
@@ -5944,9 +5909,7 @@
       <c r="Y42" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="Z42" s="8" t="s">
-        <v>422</v>
-      </c>
+      <c r="Z42" s="8"/>
       <c r="AA42" s="15" t="s">
         <v>318</v>
       </c>
@@ -5980,7 +5943,7 @@
         <v>292</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="J43" t="s">
         <v>134</v>
@@ -6027,9 +5990,7 @@
       <c r="Y43" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="Z43" s="8" t="s">
-        <v>422</v>
-      </c>
+      <c r="Z43" s="8"/>
       <c r="AA43" s="15" t="s">
         <v>319</v>
       </c>
@@ -6063,7 +6024,7 @@
         <v>293</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="J44" t="s">
         <v>134</v>
@@ -6110,9 +6071,7 @@
       <c r="Y44" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="Z44" s="8" t="s">
-        <v>422</v>
-      </c>
+      <c r="Z44" s="8"/>
       <c r="AA44" s="15" t="s">
         <v>320</v>
       </c>
@@ -6146,7 +6105,7 @@
         <v>294</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="J45" t="s">
         <v>134</v>
@@ -6193,9 +6152,7 @@
       <c r="Y45" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="Z45" s="8" t="s">
-        <v>422</v>
-      </c>
+      <c r="Z45" s="8"/>
       <c r="AA45" s="15" t="s">
         <v>321</v>
       </c>
@@ -6229,7 +6186,7 @@
         <v>252</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="J46" t="s">
         <v>134</v>
@@ -6300,7 +6257,7 @@
         <v>253</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="J47" t="s">
         <v>134</v>
@@ -6371,7 +6328,7 @@
         <v>254</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="J48" t="s">
         <v>134</v>
@@ -6439,7 +6396,7 @@
         <v>255</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="J49" t="s">
         <v>134</v>
@@ -6510,7 +6467,7 @@
         <v>256</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="J50" t="s">
         <v>134</v>
@@ -6578,7 +6535,7 @@
         <v>257</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="J51" t="s">
         <v>134</v>
@@ -6649,7 +6606,7 @@
         <v>258</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="J52" t="s">
         <v>134</v>
@@ -6720,7 +6677,7 @@
         <v>387</v>
       </c>
       <c r="I53" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="J53" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Update file excel and datasets
</commit_message>
<xml_diff>
--- a/data-raw/sites_list.xlsx
+++ b/data-raw/sites_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Itineris\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\costy\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2ED003-A9BE-41FF-B268-D181DE21700E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EA5A70-D121-44EB-8357-2EFAA702345B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1410,15 +1410,6 @@
     <t>The dataset provides the date when the vegetation growing season starts in the time profile of the Plant Phenology Index. The start-of-season occurs, by definition, when the Plant Phenology Index value reaches 25% of the season amplitude during the green-up period.  The Plant Phenology Index is a physically based vegetation index for improved monitoring of plant phenology based on Sentinel 2 images.</t>
   </si>
   <si>
-    <t>rx</t>
-  </si>
-  <si>
-    <t>ini_chl_ts</t>
-  </si>
-  <si>
-    <t>init_chl_cs</t>
-  </si>
-  <si>
     <t>/home/jovyan/itineris-dataspace/VRE_EV/DATI/EOBS_tg_9b1d144a-dc37-4b0e-8cda-1dda1d7667da_cut.nc</t>
   </si>
   <si>
@@ -1591,6 +1582,15 @@
   </si>
   <si>
     <t>/home/jovyan/itineris-dataspace/VRE_EV/DATI/Water chemistry_Lago Maggiore_Italy.csv</t>
+  </si>
+  <si>
+    <t>tx</t>
+  </si>
+  <si>
+    <t>int_chl_ts</t>
+  </si>
+  <si>
+    <t>int_chl_cs</t>
   </si>
 </sst>
 </file>
@@ -2538,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77B816B-8EFB-A44F-8A3F-6C6CC0FEF266}">
   <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Z38" sqref="Z38"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AA25" sqref="AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2683,7 +2683,7 @@
         <v>88</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="J2" t="s">
         <v>89</v>
@@ -2722,7 +2722,7 @@
         <v>91</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="J3" t="s">
         <v>99</v>
@@ -2767,7 +2767,7 @@
         <v>379</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="J4" t="s">
         <v>89</v>
@@ -2841,7 +2841,7 @@
         <v>115</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="J5" t="s">
         <v>134</v>
@@ -2889,7 +2889,7 @@
         <v>297</v>
       </c>
       <c r="Z5" s="8" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="AA5" t="s">
         <v>302</v>
@@ -2924,7 +2924,7 @@
         <v>114</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="J6" t="s">
         <v>134</v>
@@ -2972,7 +2972,7 @@
         <v>298</v>
       </c>
       <c r="Z6" s="8" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="AA6" s="15" t="s">
         <v>322</v>
@@ -3007,7 +3007,7 @@
         <v>113</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="J7" t="s">
         <v>134</v>
@@ -3055,10 +3055,10 @@
         <v>299</v>
       </c>
       <c r="Z7" s="8" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="AA7" s="15" t="s">
-        <v>411</v>
+        <v>469</v>
       </c>
       <c r="AB7">
         <v>1</v>
@@ -3090,7 +3090,7 @@
         <v>112</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="J8" t="s">
         <v>134</v>
@@ -3138,7 +3138,7 @@
         <v>300</v>
       </c>
       <c r="Z8" s="8" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="AA8" s="15" t="s">
         <v>303</v>
@@ -3173,7 +3173,7 @@
         <v>111</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="J9" t="s">
         <v>134</v>
@@ -3221,7 +3221,7 @@
         <v>301</v>
       </c>
       <c r="Z9" s="8" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="AA9" s="15" t="s">
         <v>304</v>
@@ -3256,7 +3256,7 @@
         <v>110</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="J10" t="s">
         <v>135</v>
@@ -3327,7 +3327,7 @@
         <v>249</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="J11" t="s">
         <v>134</v>
@@ -3398,7 +3398,7 @@
         <v>117</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="J12" t="s">
         <v>339</v>
@@ -3446,7 +3446,7 @@
         <v>338</v>
       </c>
       <c r="Z12" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA12" s="15" t="s">
         <v>323</v>
@@ -3481,7 +3481,7 @@
         <v>118</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="J13" t="s">
         <v>134</v>
@@ -3529,7 +3529,7 @@
         <v>338</v>
       </c>
       <c r="Z13" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA13" s="15" t="s">
         <v>326</v>
@@ -3564,7 +3564,7 @@
         <v>119</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="J14" t="s">
         <v>134</v>
@@ -3612,7 +3612,7 @@
         <v>338</v>
       </c>
       <c r="Z14" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA14" s="15" t="s">
         <v>331</v>
@@ -3647,7 +3647,7 @@
         <v>120</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J15" t="s">
         <v>134</v>
@@ -3695,10 +3695,10 @@
         <v>338</v>
       </c>
       <c r="Z15" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA15" s="15" t="s">
-        <v>412</v>
+        <v>470</v>
       </c>
       <c r="AB15">
         <v>1</v>
@@ -3730,7 +3730,7 @@
         <v>121</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="J16" t="s">
         <v>134</v>
@@ -3778,7 +3778,7 @@
         <v>338</v>
       </c>
       <c r="Z16" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA16" s="15" t="s">
         <v>332</v>
@@ -3813,7 +3813,7 @@
         <v>122</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="J17" t="s">
         <v>134</v>
@@ -3861,7 +3861,7 @@
         <v>338</v>
       </c>
       <c r="Z17" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA17" s="15" t="s">
         <v>324</v>
@@ -3896,7 +3896,7 @@
         <v>123</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="J18" t="s">
         <v>134</v>
@@ -3944,7 +3944,7 @@
         <v>338</v>
       </c>
       <c r="Z18" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA18" s="15" t="s">
         <v>327</v>
@@ -3979,7 +3979,7 @@
         <v>124</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="J19" t="s">
         <v>134</v>
@@ -4027,7 +4027,7 @@
         <v>338</v>
       </c>
       <c r="Z19" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA19" s="15" t="s">
         <v>328</v>
@@ -4062,7 +4062,7 @@
         <v>125</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="J20" t="s">
         <v>134</v>
@@ -4110,10 +4110,10 @@
         <v>338</v>
       </c>
       <c r="Z20" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA20" s="14" t="s">
-        <v>413</v>
+        <v>471</v>
       </c>
       <c r="AB20">
         <v>1</v>
@@ -4145,7 +4145,7 @@
         <v>126</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="J21" t="s">
         <v>134</v>
@@ -4193,7 +4193,7 @@
         <v>338</v>
       </c>
       <c r="Z21" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA21" s="15" t="s">
         <v>333</v>
@@ -4228,7 +4228,7 @@
         <v>127</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="J22" t="s">
         <v>134</v>
@@ -4276,7 +4276,7 @@
         <v>338</v>
       </c>
       <c r="Z22" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA22" s="15" t="s">
         <v>325</v>
@@ -4311,7 +4311,7 @@
         <v>128</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="J23" t="s">
         <v>134</v>
@@ -4359,7 +4359,7 @@
         <v>338</v>
       </c>
       <c r="Z23" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA23" s="15" t="s">
         <v>329</v>
@@ -4394,7 +4394,7 @@
         <v>129</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="J24" t="s">
         <v>134</v>
@@ -4442,7 +4442,7 @@
         <v>338</v>
       </c>
       <c r="Z24" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA24" s="15" t="s">
         <v>330</v>
@@ -4477,7 +4477,7 @@
         <v>130</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="J25" t="s">
         <v>134</v>
@@ -4525,7 +4525,7 @@
         <v>338</v>
       </c>
       <c r="Z25" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA25" s="15" t="s">
         <v>335</v>
@@ -4560,7 +4560,7 @@
         <v>131</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="J26" t="s">
         <v>134</v>
@@ -4608,7 +4608,7 @@
         <v>338</v>
       </c>
       <c r="Z26" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA26" s="15" t="s">
         <v>334</v>
@@ -4643,7 +4643,7 @@
         <v>132</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="J27" t="s">
         <v>134</v>
@@ -4691,7 +4691,7 @@
         <v>338</v>
       </c>
       <c r="Z27" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA27" s="15" t="s">
         <v>336</v>
@@ -4726,7 +4726,7 @@
         <v>133</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="J28" t="s">
         <v>134</v>
@@ -4774,7 +4774,7 @@
         <v>338</v>
       </c>
       <c r="Z28" s="8" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="AA28" s="15" t="s">
         <v>337</v>
@@ -4809,7 +4809,7 @@
         <v>278</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="J29" t="s">
         <v>134</v>
@@ -4890,7 +4890,7 @@
         <v>279</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="J30" t="s">
         <v>134</v>
@@ -4971,7 +4971,7 @@
         <v>280</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="J31" t="s">
         <v>134</v>
@@ -5052,7 +5052,7 @@
         <v>281</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="J32" t="s">
         <v>134</v>
@@ -5133,7 +5133,7 @@
         <v>282</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="J33" t="s">
         <v>134</v>
@@ -5214,7 +5214,7 @@
         <v>283</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="J34" t="s">
         <v>134</v>
@@ -5295,7 +5295,7 @@
         <v>284</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="J35" t="s">
         <v>134</v>
@@ -5376,7 +5376,7 @@
         <v>285</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="J36" t="s">
         <v>134</v>
@@ -5457,7 +5457,7 @@
         <v>286</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="J37" t="s">
         <v>134</v>
@@ -5538,7 +5538,7 @@
         <v>287</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="J38" t="s">
         <v>134</v>
@@ -5619,7 +5619,7 @@
         <v>288</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="J39" t="s">
         <v>134</v>
@@ -5700,7 +5700,7 @@
         <v>289</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="J40" t="s">
         <v>134</v>
@@ -5781,7 +5781,7 @@
         <v>290</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="J41" t="s">
         <v>134</v>
@@ -5862,7 +5862,7 @@
         <v>291</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="J42" t="s">
         <v>134</v>
@@ -5943,7 +5943,7 @@
         <v>292</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="J43" t="s">
         <v>134</v>
@@ -6024,7 +6024,7 @@
         <v>293</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="J44" t="s">
         <v>134</v>
@@ -6105,7 +6105,7 @@
         <v>294</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="J45" t="s">
         <v>134</v>
@@ -6186,7 +6186,7 @@
         <v>252</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="J46" t="s">
         <v>134</v>
@@ -6257,7 +6257,7 @@
         <v>253</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="J47" t="s">
         <v>134</v>
@@ -6328,7 +6328,7 @@
         <v>254</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="J48" t="s">
         <v>134</v>
@@ -6396,7 +6396,7 @@
         <v>255</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="J49" t="s">
         <v>134</v>
@@ -6467,7 +6467,7 @@
         <v>256</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="J50" t="s">
         <v>134</v>
@@ -6535,7 +6535,7 @@
         <v>257</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="J51" t="s">
         <v>134</v>
@@ -6606,7 +6606,7 @@
         <v>258</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="J52" t="s">
         <v>134</v>
@@ -6677,7 +6677,7 @@
         <v>387</v>
       </c>
       <c r="I53" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="J53" t="s">
         <v>89</v>

</xml_diff>